<commit_message>
Updates on the solar part of the power network file
</commit_message>
<xml_diff>
--- a/Mini-projet-trey_Buchser_Joye/data/power_profile.xlsx
+++ b/Mini-projet-trey_Buchser_Joye/data/power_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\micael\git\rhtlab_MIB\Mini-projet-trey_Buchser_Joye\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999A3EA-0C38-4710-B0E5-CAC27C658E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9837201B-9582-4E05-94E5-9853D4282EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="load" sheetId="5" r:id="rId1"/>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:BT98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AY8" sqref="AY8"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17178,11 +17178,14 @@
     <protectedRange sqref="B3:AP98" name="Plage1_1_1"/>
   </protectedRanges>
   <mergeCells count="25">
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -17195,14 +17198,11 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17210,10 +17210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0724F9-1790-4ECA-B4EA-D773CFA5B42B}">
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AM98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17424,124 +17424,2796 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>8.3333333333333301E-2</v>
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>0.16666666666666699</v>
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>0.20833333333333301</v>
+        <v>5.2083333333333301E-2</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>0.25</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>0.29166666666666702</v>
+        <v>7.2916666666666699E-2</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>0.33333333333333298</v>
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>0.375</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>0.41666666666666702</v>
+        <v>0.104166666666667</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>0.45833333333333298</v>
+        <v>0.114583333333333</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>0.5</v>
+        <v>0.125</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.14583333333333301</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.15625</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.17708333333333301</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.1875</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>0.19791666666666699</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.51365527499999553</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1.0273105499999919</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>0.21875</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1.540965824999988</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.45819869999999602</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0.22916666666666699</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2.054621099999983</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.91639739999999326</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>0.23958333333333301</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>3.8854799874999739</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1.3745960999999891</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>5.7163388750000026</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1.832794799999985</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>0.26041666666666702</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>7.5471977625000353</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>3.5308524499999758</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>0.27083333333333298</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>9.378056650000083</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>5.228910100000002</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>0.28125</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>11.908692881250071</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>6.9269677500000331</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>14.439329112500049</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>8.6250254000000819</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>0.30208333333333298</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>16.969965343750019</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>11.18826172500007</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>19.500601575000001</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>13.75149805000005</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="B34">
+        <v>3.5768706249999768E-2</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>21.867990731249989</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>16.314734375000022</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B35">
+        <v>7.1537412499999342E-2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>24.23537988749996</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>18.877970699999999</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="B36">
+        <v>0.1073061187499991</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>26.602769043749941</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>21.176808593749989</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>0.35416666666666702</v>
+      </c>
+      <c r="B37">
+        <v>0.14307482499999891</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>28.970158199999918</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>23.475646487499962</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="B38">
+        <v>1.7389414937499701</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>31.13125341874996</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0.5244137562499902</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>25.774484381249941</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="B39">
+        <v>3.3348081624999999</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>33.292348637499998</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1.0488275124999999</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>28.073322274999921</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>0.38541666666666702</v>
+      </c>
+      <c r="B40">
+        <v>4.9306748312500286</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>35.45344385625004</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1.5732412687500099</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>30.06023389374996</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="B41">
+        <v>6.5265415000000413</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>37.614539075000039</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>2.097655025000015</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>32.047145512500002</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="B42">
+        <v>7.8181661375000333</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>38.703405281250028</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>2.5890765937500122</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>34.034057131250037</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B43">
+        <v>9.1097907750000253</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>39.792271487500017</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>3.080498162500009</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>36.020968750000058</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="B44">
+        <v>10.401415412500009</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>40.881137693750013</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>3.5719197312500031</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>37.718104493750047</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="B45">
+        <v>11.69304005</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>41.970003900000002</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>4.0633413000000003</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>39.415240237500029</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>0.44791666666666702</v>
+      </c>
+      <c r="B46">
+        <v>13.406195074999991</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>42.486155268749997</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>4.2947477937499992</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>41.112375981250011</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B47">
+        <v>15.11935009999997</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>43.002306637499991</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>4.5261542874999963</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>42.809511725</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="B48">
+        <v>16.832505124999951</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>43.518458006249993</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>4.7575607812499943</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>43.62370215624999</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>0.47916666666666702</v>
+      </c>
+      <c r="B49">
+        <v>18.54566014999995</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>44.034609374999988</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>4.9889672749999932</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>44.437892587499981</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="B50">
+        <v>17.983342525000008</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>44.652867187499993</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>5.0990180562499976</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>45.252083018749978</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B51">
+        <v>17.421024899999999</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>45.271124999999998</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>5.2090688375000003</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>46.066273449999969</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>0.51041666666666696</v>
+      </c>
+      <c r="B52">
+        <v>16.85870727499999</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>45.88938281250001</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>5.3191196187500012</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>46.192474618749998</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="B53">
+        <v>16.296389649999941</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>46.507640624999993</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>5.4291703999999967</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>46.318675787499998</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="B54">
+        <v>14.374237549999959</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>46.112312499999987</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>5.3179660562499977</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>46.444876956249999</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>0.54166666666666696</v>
       </c>
+      <c r="B55">
+        <v>12.452085449999981</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>45.716984375000003</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>5.2067617124999996</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>46.571078124999993</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="B56">
+        <v>10.529933349999981</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>45.321656249999997</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>5.0955573687499998</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>46.101112306249988</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="B57">
+        <v>8.6077812500000004</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>44.926328124999998</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>4.9843530250000008</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>45.63114648749999</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>0.57291666666666696</v>
+      </c>
+      <c r="B58">
+        <v>8.7527277812499982</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>43.689188475000023</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>4.7139557500000038</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>45.161180668749992</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>0.58333333333333304</v>
       </c>
+      <c r="B59">
+        <v>8.8976743124999995</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>42.452048825000013</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>4.4435584750000032</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>44.691214849999987</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="B60">
+        <v>9.0426208437499973</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>41.214909175000031</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>4.1731612000000062</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>44.153650393750013</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="B61">
+        <v>9.1875673749999951</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>39.977769525000042</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>3.9027639250000088</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>43.616085937500003</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="B62">
+        <v>8.3259988937500093</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>39.41670019375001</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>3.4441038250000049</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>43.078521481250007</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>0.625</v>
       </c>
+      <c r="B63">
+        <v>7.4644304125000014</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>38.855630862500007</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>2.9854437250000001</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>42.540957025000019</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>0.63541666666666696</v>
+      </c>
+      <c r="B64">
+        <v>6.6028619312499908</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>38.294561531249997</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>2.5267836249999949</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>40.609186518750022</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="B65">
+        <v>5.7412934499999571</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>37.733492199999937</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>2.068123524999983</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>38.677416012499997</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="B66">
+        <v>4.4188910687499714</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>35.91802246874996</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>1.551092643749989</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>36.745645506249993</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
         <v>0.66666666666666696</v>
       </c>
+      <c r="B67">
+        <v>3.0964886874999862</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>34.102552737499977</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>1.0340617624999939</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>34.813874999999953</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>0.67708333333333304</v>
+      </c>
+      <c r="B68">
+        <v>1.7740863062499861</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>32.287083006249979</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0.51703088124999441</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>33.040834962499957</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="B69">
+        <v>0.45168392499999999</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>30.471613274999999</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>31.267794924999979</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>0.69791666666666696</v>
+      </c>
+      <c r="B70">
+        <v>0.33876294375000121</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>27.977577631250028</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>29.49475488749998</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>0.70833333333333304</v>
       </c>
+      <c r="B71">
+        <v>0.22584196250000119</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>25.483541987500029</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>27.721714850000001</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="B72">
+        <v>0.1129209812500024</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>22.989506343750051</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>25.484246587500021</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>0.72916666666666696</v>
+      </c>
+      <c r="B73">
+        <v>3.6082248300317588E-15</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>20.49547070000008</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>23.246778325000019</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>0.73958333333333304</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>18.08856908750003</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>21.009310062500049</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>0.75</v>
       </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>15.681667474999999</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>18.771841800000072</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>0.76041666666666696</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>13.274765862499979</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>16.321886231250019</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>0.77083333333333304</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>10.86786424999994</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>13.871930662500001</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>9.0340941687499612</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>11.421975093749969</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>0.79166666666666696</v>
       </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>7.2003240874999808</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>8.9720195249999506</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>0.80208333333333304</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>5.3665540062499808</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>7.4409991437499681</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>3.5327839249999999</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>5.9099787624999838</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>0.82291666666666696</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>2.6495879437500101</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>4.3789583812499844</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>0.83333333333333304</v>
       </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>1.76639196250001</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>2.8479380000000001</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0.88319598125001875</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>2.1359535000000069</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>0.85416666666666696</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>2.7977620220553939E-14</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>1.423969000000008</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>0.86458333333333304</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0.71198450000001534</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
         <v>0.875</v>
       </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>2.3092638912203259E-14</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>0.88541666666666696</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>0.89583333333333304</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>0.90625</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
         <v>0.91666666666666696</v>
       </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>0.92708333333333304</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>0.94791666666666696</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
         <v>0.95833333333333304</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>0.96875</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>0.97916666666666696</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>0.98958333333333304</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -17554,14 +20226,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>